<commit_message>
added more runs on x86_64 spreadsheet
</commit_message>
<xml_diff>
--- a/docs/x86_64_benchmarks/x86_64_float_double_comparison.xlsx
+++ b/docs/x86_64_benchmarks/x86_64_float_double_comparison.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t xml:space="preserve">Float</t>
   </si>
@@ -41,6 +41,21 @@
   </si>
   <si>
     <t xml:space="preserve">Run 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run 10</t>
   </si>
   <si>
     <t xml:space="preserve">AVG</t>
@@ -156,16 +171,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="K24" activeCellId="0" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -194,7 +206,22 @@
       <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
@@ -216,8 +243,23 @@
         <v>635</v>
       </c>
       <c r="G3" s="0" t="n">
-        <f aca="false">AVERAGE(B3:F3)</f>
-        <v>663</v>
+        <v>620</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>626</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>629</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>644</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>668</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <f aca="false">AVERAGE(B3:K3)</f>
+        <v>650.2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -240,8 +282,23 @@
         <v>3354</v>
       </c>
       <c r="G4" s="0" t="n">
-        <f aca="false">AVERAGE(B4:F4)</f>
-        <v>3520.2</v>
+        <v>2531</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>2773</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>3327</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>3499</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>2770</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <f aca="false">AVERAGE(B4:K4)</f>
+        <v>3250.1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -264,8 +321,23 @@
         <v>31983</v>
       </c>
       <c r="G5" s="0" t="n">
-        <f aca="false">AVERAGE(B5:F5)</f>
-        <v>31734.4</v>
+        <v>33014</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>32494</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>32887</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>31448</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>28175</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <f aca="false">AVERAGE(B5:K5)</f>
+        <v>31669</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -288,8 +360,23 @@
         <v>4619</v>
       </c>
       <c r="G6" s="0" t="n">
-        <f aca="false">AVERAGE(B6:F6)</f>
-        <v>4247</v>
+        <v>3726</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>4597</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>3998</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>3593</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>3530</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <f aca="false">AVERAGE(B6:K6)</f>
+        <v>4067.9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -312,8 +399,23 @@
         <v>973</v>
       </c>
       <c r="G7" s="0" t="n">
-        <f aca="false">AVERAGE(B7:F7)</f>
-        <v>876.4</v>
+        <v>738</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>753</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>762</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>853</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>705</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <f aca="false">AVERAGE(B7:K7)</f>
+        <v>819.3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -336,8 +438,23 @@
         <v>208</v>
       </c>
       <c r="G8" s="0" t="n">
-        <f aca="false">AVERAGE(B8:F8)</f>
-        <v>201.8</v>
+        <v>175</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>175</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>175</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <f aca="false">AVERAGE(B8:K8)</f>
+        <v>213.4</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -360,8 +477,23 @@
         <v>40</v>
       </c>
       <c r="G9" s="0" t="n">
-        <f aca="false">AVERAGE(B9:F9)</f>
-        <v>36.4</v>
+        <v>30</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <f aca="false">AVERAGE(B9:K9)</f>
+        <v>36.1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -384,13 +516,28 @@
         <v>636</v>
       </c>
       <c r="G10" s="0" t="n">
-        <f aca="false">AVERAGE(B10:F10)</f>
-        <v>689.8</v>
+        <v>692</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>766</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>771</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>692</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <f aca="false">AVERAGE(B10:K10)</f>
+        <v>712</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">SUM(B3:B10)</f>
@@ -413,13 +560,33 @@
         <v>42448</v>
       </c>
       <c r="G11" s="0" t="n">
-        <f aca="false">AVERAGE(B11:F11)</f>
-        <v>41969</v>
+        <f aca="false">SUM(G3:G10)</f>
+        <v>41526</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <f aca="false">SUM(H3:H10)</f>
+        <v>42446</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <f aca="false">SUM(I3:I10)</f>
+        <v>42604</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <f aca="false">SUM(J3:J10)</f>
+        <v>40989</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <f aca="false">SUM(K3:K10)</f>
+        <v>36770</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <f aca="false">AVERAGE(B11:K11)</f>
+        <v>41418</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -444,6 +611,21 @@
       <c r="G15" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="H15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
@@ -465,8 +647,23 @@
         <v>535</v>
       </c>
       <c r="G16" s="0" t="n">
-        <f aca="false">AVERAGE(B16:F16)</f>
-        <v>567.4</v>
+        <v>599</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>596</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>526</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>590</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>617</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <f aca="false">AVERAGE(B16:K16)</f>
+        <v>576.5</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -489,8 +686,23 @@
         <v>2625</v>
       </c>
       <c r="G17" s="0" t="n">
-        <f aca="false">AVERAGE(B17:F17)</f>
-        <v>2850.2</v>
+        <v>3045</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>3372</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>2589</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>24779</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>3342</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <f aca="false">AVERAGE(B17:K17)</f>
+        <v>5137.8</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -513,8 +725,23 @@
         <v>27631</v>
       </c>
       <c r="G18" s="0" t="n">
-        <f aca="false">AVERAGE(B18:F18)</f>
-        <v>32163.2</v>
+        <v>31898</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>31085</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>33897</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>28608</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <v>33698</v>
+      </c>
+      <c r="L18" s="0" t="n">
+        <f aca="false">AVERAGE(B18:K18)</f>
+        <v>32000.2</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -537,8 +764,23 @@
         <v>3826</v>
       </c>
       <c r="G19" s="0" t="n">
-        <f aca="false">AVERAGE(B19:F19)</f>
-        <v>4505.6</v>
+        <v>3656</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>3662</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>4025</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>3941</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>3765</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <f aca="false">AVERAGE(B19:K19)</f>
+        <v>4157.7</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -561,8 +803,23 @@
         <v>336</v>
       </c>
       <c r="G20" s="0" t="n">
-        <f aca="false">AVERAGE(B20:F20)</f>
-        <v>309.6</v>
+        <v>478</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>293</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>242</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>254</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <v>288</v>
+      </c>
+      <c r="L20" s="0" t="n">
+        <f aca="false">AVERAGE(B20:K20)</f>
+        <v>310.3</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -585,8 +842,23 @@
         <v>224</v>
       </c>
       <c r="G21" s="0" t="n">
-        <f aca="false">AVERAGE(B21:F21)</f>
-        <v>299.4</v>
+        <v>233</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>209</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>194</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <v>194</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="L21" s="0" t="n">
+        <f aca="false">AVERAGE(B21:K21)</f>
+        <v>252.7</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -609,8 +881,23 @@
         <v>58</v>
       </c>
       <c r="G22" s="0" t="n">
-        <f aca="false">AVERAGE(B22:F22)</f>
-        <v>48.2</v>
+        <v>70</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="L22" s="0" t="n">
+        <f aca="false">AVERAGE(B22:K22)</f>
+        <v>47.7</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -633,13 +920,28 @@
         <v>753</v>
       </c>
       <c r="G23" s="0" t="n">
-        <f aca="false">AVERAGE(B23:F23)</f>
-        <v>741.4</v>
+        <v>726</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>626</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>865</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <v>774</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>774</v>
+      </c>
+      <c r="L23" s="0" t="n">
+        <f aca="false">AVERAGE(B23:K23)</f>
+        <v>747.2</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B24" s="0" t="n">
         <f aca="false">SUM(B16:B23)</f>
@@ -662,8 +964,28 @@
         <v>35988</v>
       </c>
       <c r="G24" s="0" t="n">
-        <f aca="false">AVERAGE(B24:F24)</f>
-        <v>41485</v>
+        <f aca="false">SUM(G16:G23)</f>
+        <v>40705</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <f aca="false">SUM(H16:H23)</f>
+        <v>39879</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <f aca="false">SUM(I16:I23)</f>
+        <v>42377</v>
+      </c>
+      <c r="J24" s="0" t="n">
+        <f aca="false">SUM(J16:J23)</f>
+        <v>59198</v>
+      </c>
+      <c r="K24" s="0" t="n">
+        <f aca="false">SUM(K16:K23)</f>
+        <v>42717</v>
+      </c>
+      <c r="L24" s="0" t="n">
+        <f aca="false">AVERAGE(B24:K24)</f>
+        <v>43230.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>